<commit_message>
Updated Logic to create car id dynamically. Will reduce potential overwrite issues.
</commit_message>
<xml_diff>
--- a/CAR_PERF_DATA.xlsx
+++ b/CAR_PERF_DATA.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
   <si>
     <t>CAR_CODE</t>
   </si>
@@ -321,6 +321,39 @@
   </si>
   <si>
     <t>Soft</t>
+  </si>
+  <si>
+    <t>Cayenne</t>
+  </si>
+  <si>
+    <t>GTS</t>
+  </si>
+  <si>
+    <t>SUV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>AWD</t>
+  </si>
+  <si>
+    <t>DRY_WEIGHT_UOM</t>
+  </si>
+  <si>
+    <t>LBS</t>
+  </si>
+  <si>
+    <t>10011010</t>
+  </si>
+  <si>
+    <t>10011110</t>
+  </si>
+  <si>
+    <t>10011210</t>
   </si>
 </sst>
 </file>
@@ -646,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,8 +763,8 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>10001</v>
+      <c r="A2" t="s">
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -759,8 +792,8 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10001</v>
+      <c r="A3" t="s">
+        <v>106</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
@@ -788,8 +821,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>10002</v>
+      <c r="A4" t="s">
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -817,8 +850,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>10002</v>
+      <c r="A5" t="s">
+        <v>107</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -843,6 +876,38 @@
       </c>
       <c r="Q5">
         <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6">
+        <v>405</v>
+      </c>
+      <c r="E6">
+        <v>6500</v>
+      </c>
+      <c r="F6">
+        <v>369</v>
+      </c>
+      <c r="H6">
+        <v>3500</v>
+      </c>
+      <c r="I6">
+        <v>5.5</v>
+      </c>
+      <c r="K6">
+        <v>159</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -852,10 +917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO3"/>
+  <dimension ref="A1:AP4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -901,7 +966,7 @@
     <col min="41" max="41" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1025,17 +1090,31 @@
       <c r="AO1" t="s">
         <v>82</v>
       </c>
+      <c r="AP1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>10001</v>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>CONCATENATE(B2,D2,F2)</f>
+        <v>10011010</v>
+      </c>
+      <c r="B2">
+        <f>VLOOKUP(C2,X_MAKE_D!A:B,2,FALSE)</f>
+        <v>1001</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
       </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
       <c r="E2">
         <v>911</v>
       </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
       <c r="G2" t="s">
         <v>38</v>
       </c>
@@ -1129,17 +1208,31 @@
       <c r="AO2">
         <v>3042</v>
       </c>
+      <c r="AP2" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10002</v>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A4" si="0">CONCATENATE(B3,D3,F3)</f>
+        <v>10011110</v>
+      </c>
+      <c r="B3">
+        <f>VLOOKUP(C3,X_MAKE_D!A:B,2,FALSE)</f>
+        <v>1001</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
       <c r="E3" t="s">
         <v>83</v>
       </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
       <c r="G3" t="s">
         <v>84</v>
       </c>
@@ -1238,6 +1331,103 @@
       </c>
       <c r="AO3">
         <v>2888</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>10011210</v>
+      </c>
+      <c r="B4">
+        <f>VLOOKUP(C4,X_MAKE_D!A:B,2,FALSE)</f>
+        <v>1001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4">
+        <v>2009</v>
+      </c>
+      <c r="J4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>4.8</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" t="s">
+        <v>103</v>
+      </c>
+      <c r="T4">
+        <v>4</v>
+      </c>
+      <c r="U4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z4">
+        <v>6</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD4">
+        <v>7</v>
+      </c>
+      <c r="AE4">
+        <v>70195</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO4">
+        <v>5300</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1440,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1280,6 +1470,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
@@ -1294,6 +1487,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>85</v>
       </c>
@@ -1308,6 +1504,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>91</v>
       </c>
@@ -1322,6 +1521,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
@@ -1342,12 +1544,12 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -1359,10 +1561,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
@@ -1387,8 +1589,14 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="A2" t="s">
         <v>37</v>
+      </c>
+      <c r="B2">
+        <v>1001</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
Updated logic again and tested with new row.
</commit_message>
<xml_diff>
--- a/CAR_PERF_DATA.xlsx
+++ b/CAR_PERF_DATA.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
   <si>
     <t>CAR_CODE</t>
   </si>
@@ -347,13 +347,13 @@
     <t>LBS</t>
   </si>
   <si>
-    <t>10011010</t>
-  </si>
-  <si>
-    <t>10011110</t>
-  </si>
-  <si>
-    <t>10011210</t>
+    <t>10.5:1</t>
+  </si>
+  <si>
+    <t>100112102015</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -398,9 +398,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -679,15 +680,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
@@ -763,8 +764,8 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>106</v>
+      <c r="A2" s="2">
+        <v>100110102015</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -792,8 +793,8 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>106</v>
+      <c r="A3" s="2">
+        <v>100110102015</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
@@ -821,8 +822,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>107</v>
+      <c r="A4" s="2">
+        <v>100111102015</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -850,8 +851,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>107</v>
+      <c r="A5" s="2">
+        <v>100111102015</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -879,8 +880,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>108</v>
+      <c r="A6" s="2">
+        <v>100112102009</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -908,6 +909,35 @@
       </c>
       <c r="Q6">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7">
+        <v>440</v>
+      </c>
+      <c r="E7">
+        <v>6000</v>
+      </c>
+      <c r="F7">
+        <v>442</v>
+      </c>
+      <c r="I7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K7">
+        <v>163</v>
+      </c>
+      <c r="P7">
+        <v>15</v>
+      </c>
+      <c r="Q7">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -917,15 +947,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP4"/>
+  <dimension ref="A1:AP5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
@@ -1096,8 +1126,8 @@
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>CONCATENATE(B2,D2,F2)</f>
-        <v>10011010</v>
+        <f>CONCATENATE(B2,D2,F2,H2)</f>
+        <v>100110102015</v>
       </c>
       <c r="B2">
         <f>VLOOKUP(C2,X_MAKE_D!A:B,2,FALSE)</f>
@@ -1214,8 +1244,8 @@
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A4" si="0">CONCATENATE(B3,D3,F3)</f>
-        <v>10011110</v>
+        <f t="shared" ref="A3:A5" si="0">CONCATENATE(B3,D3,F3,H3)</f>
+        <v>100111102015</v>
       </c>
       <c r="B3">
         <f>VLOOKUP(C3,X_MAKE_D!A:B,2,FALSE)</f>
@@ -1339,7 +1369,7 @@
     <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>10011210</v>
+        <v>100112102009</v>
       </c>
       <c r="B4">
         <f>VLOOKUP(C4,X_MAKE_D!A:B,2,FALSE)</f>
@@ -1387,9 +1417,6 @@
       <c r="Q4" t="s">
         <v>42</v>
       </c>
-      <c r="R4" t="s">
-        <v>68</v>
-      </c>
       <c r="S4" t="s">
         <v>103</v>
       </c>
@@ -1409,13 +1436,13 @@
         <v>6</v>
       </c>
       <c r="AA4" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="AB4">
+        <v>6</v>
       </c>
       <c r="AC4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD4">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="AE4">
         <v>70195</v>
@@ -1428,6 +1455,115 @@
       </c>
       <c r="AP4" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>100112102015</v>
+      </c>
+      <c r="B5">
+        <f>VLOOKUP(C5,X_MAKE_D!A:B,2,FALSE)</f>
+        <v>1001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5">
+        <v>2015</v>
+      </c>
+      <c r="J5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
+      </c>
+      <c r="P5">
+        <v>3.6</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" t="s">
+        <v>106</v>
+      </c>
+      <c r="S5" t="s">
+        <v>103</v>
+      </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
+      <c r="U5" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB5">
+        <v>7</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE5">
+        <v>95500</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG5">
+        <v>66.5</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI5">
+        <v>85.2</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK5">
+        <v>113.98</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM5">
+        <v>191.14</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new column: FUEL_TYPE
</commit_message>
<xml_diff>
--- a/CAR_PERF_DATA.xlsx
+++ b/CAR_PERF_DATA.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="111">
   <si>
     <t>CAR_CODE</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>FUEL_TYPE</t>
+  </si>
+  <si>
+    <t>Premium</t>
   </si>
 </sst>
 </file>
@@ -682,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -947,10 +953,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP5"/>
+  <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,30 +979,31 @@
     <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="22.1640625" customWidth="1"/>
-    <col min="25" max="25" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="22.1640625" customWidth="1"/>
+    <col min="26" max="26" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1052,79 +1059,82 @@
         <v>67</v>
       </c>
       <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>69</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>70</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>71</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>72</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>73</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>58</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>59</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>60</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>61</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>62</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>63</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>82</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>CONCATENATE(B2,D2,F2,H2)</f>
         <v>100110102015</v>
@@ -1179,70 +1189,73 @@
         <v>68</v>
       </c>
       <c r="S2" t="s">
+        <v>110</v>
+      </c>
+      <c r="T2" t="s">
         <v>43</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>2</v>
       </c>
-      <c r="U2" t="s">
-        <v>40</v>
-      </c>
       <c r="V2" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="W2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" t="s">
         <v>44</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>7</v>
       </c>
-      <c r="AA2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AB2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" t="s">
         <v>44</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>7</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>84300</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>49</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>51.3</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>64</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>71.180000000000007</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>64</v>
       </c>
-      <c r="AK2">
+      <c r="AL2">
         <v>176.81</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>64</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>96.46</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>64</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
         <v>3042</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="0">CONCATENATE(B3,D3,F3,H3)</f>
         <v>100111102015</v>
@@ -1297,76 +1310,79 @@
         <v>68</v>
       </c>
       <c r="S3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T3" t="s">
         <v>43</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>2</v>
       </c>
-      <c r="U3" t="s">
-        <v>40</v>
-      </c>
       <c r="V3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" t="s">
         <v>44</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>96</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>97</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>44</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>6</v>
       </c>
-      <c r="AA3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC3" t="s">
+      <c r="AB3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD3" t="s">
         <v>44</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>7</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>52100</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>49</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>50.5</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>64</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>70.900000000000006</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>64</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>172.2</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>64</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>97.4</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>64</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>2888</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>100112102009</v>
@@ -1418,46 +1434,49 @@
         <v>42</v>
       </c>
       <c r="S4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T4" t="s">
         <v>103</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>4</v>
       </c>
-      <c r="U4" t="s">
-        <v>40</v>
-      </c>
       <c r="V4" t="s">
         <v>40</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="W4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" t="s">
         <v>44</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>6</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>44</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>6</v>
       </c>
-      <c r="AC4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE4">
+      <c r="AD4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF4">
         <v>70195</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>49</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>5300</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>100112102015</v>
@@ -1512,57 +1531,60 @@
         <v>106</v>
       </c>
       <c r="S5" t="s">
+        <v>110</v>
+      </c>
+      <c r="T5" t="s">
         <v>103</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>4</v>
       </c>
-      <c r="U5" t="s">
-        <v>40</v>
-      </c>
       <c r="V5" t="s">
         <v>40</v>
       </c>
-      <c r="Y5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA5" t="s">
+      <c r="W5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB5" t="s">
         <v>44</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>7</v>
       </c>
-      <c r="AC5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE5">
+      <c r="AD5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF5">
         <v>95500</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>49</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>66.5</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>64</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>85.2</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>64</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>113.98</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>64</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>191.14</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>